<commit_message>
Update code, now we can redirect the output file happily.
</commit_message>
<xml_diff>
--- a/scripts/result.xlsx
+++ b/scripts/result.xlsx
@@ -345,7 +345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -356,248 +356,128 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>ap</t>
+          <t>ad</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>ap</t>
+          <t>aw</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>ap</t>
+          <t>da</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>ca</t>
+          <t>dw</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>cp</t>
+          <t>wa</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>cs</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>pa</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>pc</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>ps</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>sa</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>sc</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>sp</t>
+          <t>wd</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>0.772</t>
+          <t>0.795</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>0.916</t>
+          <t>0.825</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>0.815</t>
+          <t>0.567</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>0.725</t>
+          <t>0.926</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>0.846</t>
+          <t>0.607</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>0.783</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>0.734</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>0.493</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>0.159</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>0.413</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>0.563</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>0.325</t>
+          <t>0.982</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>0.760</t>
+          <t>0.843</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>0.919</t>
+          <t>0.815</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>0.740</t>
+          <t>0.587</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>0.726</t>
+          <t>0.897</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>0.844</t>
+          <t>0.628</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>0.780</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>0.691</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>0.532</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>0.160</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>0.488</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>0.545</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>0.334</t>
+          <t>0.974</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>0.763</t>
+          <t>0.833</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>0.918</t>
+          <t>0.824</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0.657</t>
+          <t>0.586</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.757</t>
+          <t>0.913</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>0.762</t>
+          <t>0.612</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>0.763</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>0.721</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>0.569</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>0.140</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>0.451</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>0.540</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>0.366</t>
+          <t>0.970</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Improve the technique of redirecting in DG_rotation_trainer.
</commit_message>
<xml_diff>
--- a/scripts/result.xlsx
+++ b/scripts/result.xlsx
@@ -388,59 +388,59 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>0.795</t>
+          <t>0.831</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>0.825</t>
+          <t>0.794</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>0.567</t>
+          <t>0.595</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>0.926</t>
+          <t>0.887</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>0.607</t>
+          <t>0.627</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>0.982</t>
+          <t>0.978</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>0.843</t>
+          <t>0.837</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>0.815</t>
+          <t>0.824</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>0.587</t>
+          <t>0.558</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>0.897</t>
+          <t>0.908</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>0.628</t>
+          <t>0.618</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -452,32 +452,32 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>0.833</t>
+          <t>0.841</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>0.824</t>
+          <t>0.840</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0.586</t>
+          <t>0.588</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.913</t>
+          <t>0.828</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>0.612</t>
+          <t>0.629</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>0.970</t>
+          <t>0.982</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update code to read txt to xlsx.
</commit_message>
<xml_diff>
--- a/scripts/result.xlsx
+++ b/scripts/result.xlsx
@@ -345,7 +345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -354,128 +354,1222 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>ad</t>
-        </is>
-      </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>aw</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>da</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>dw</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>wa</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>wd</t>
+          <t>0.0_0.6_0.2_0.1</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>0.831</t>
+          <t>ad</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>0.794</t>
+          <t>aw</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>0.595</t>
+          <t>da</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>0.887</t>
+          <t>dw</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>0.627</t>
+          <t>wa</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>0.978</t>
+          <t>wd</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>0.837</t>
+          <t>0.849</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>0.824</t>
+          <t>0.829</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>0.558</t>
+          <t>0.596</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>0.908</t>
+          <t>0.894</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>0.618</t>
+          <t>0.612</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>0.974</t>
+          <t>0.968</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>0.839</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>0.845</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>0.604</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>0.886</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>0.632</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>0.980</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>0.839</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>0.845</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>0.590</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>0.907</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>0.609</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>0.990</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>0.0_0.6_0.3_0.1</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>ad</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>aw</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>da</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>dw</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>wa</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>wd</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>0.823</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>0.813</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>0.590</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>0.859</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>0.604</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>0.978</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>0.819</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>0.824</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>0.585</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>0.907</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>0.603</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>0.964</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>0.833</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>0.818</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>0.593</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>0.894</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>0.608</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>0.972</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>0.0_0.6_0.4_0.1</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>ad</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>aw</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>da</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>dw</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>wa</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>wd</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>0.827</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>0.820</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>0.583</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>0.909</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>0.602</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>0.976</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>0.847</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>0.814</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>0.596</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>0.918</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>0.626</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>0.972</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>0.847</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>0.826</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>0.559</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>0.888</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>0.610</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>0.978</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>0.0_0.6_0.5_0.1</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>ad</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>aw</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>da</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>dw</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>wa</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>wd</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>0.855</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>0.815</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>0.568</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>0.893</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>0.620</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>0.970</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>0.827</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>0.816</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>0.577</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>0.889</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>0.622</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>0.964</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>0.849</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>0.813</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>0.567</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>0.912</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>0.610</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>0.974</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>0.0_0.6_0.8_0.1</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>0.4_0.6_0.7_0.1</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>ad</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>aw</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>da</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>dw</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>wa</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>wd</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>0.839</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>0.818</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>0.605</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>0.918</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>0.601</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>0.976</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>0.827</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>0.829</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>0.589</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>0.904</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>0.628</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>0.980</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>0.837</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>0.820</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>0.573</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>0.881</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>0.627</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>0.962</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>0.4_0.6_0.9_0.1</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>ad</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>aw</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>da</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>dw</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>wa</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>wd</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>0.839</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>0.815</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>0.582</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>0.892</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>0.639</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>0.978</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>0.831</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>0.826</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>0.575</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>0.889</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>0.627</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>0.970</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>0.823</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>0.803</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>0.599</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>0.879</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>0.611</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>0.988</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>0.6_0.6_0.3_0.1</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>ad</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>aw</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>da</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>dw</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>wa</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>wd</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
           <t>0.841</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>0.816</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>0.612</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>0.886</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>0.620</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>0.966</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>0.863</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>0.805</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>0.556</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>0.875</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>0.616</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>0.968</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>0.807</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>0.844</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>0.575</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>0.898</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>0.609</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>0.980</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>0.6_0.6_0.5_0.1</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>ad</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>aw</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>da</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>dw</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>wa</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>wd</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>0.831</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>0.800</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>0.586</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>0.903</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>0.625</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>0.980</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>0.843</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>0.816</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>0.589</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>0.874</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>0.618</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>0.986</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>0.827</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>0.829</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>0.567</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>0.918</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>0.619</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>0.956</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>0.6_0.6_0.7_0.1</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>ad</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>aw</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>da</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>dw</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>wa</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>wd</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>0.831</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>0.794</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>0.595</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>0.887</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>0.627</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>0.978</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>0.837</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>0.824</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>0.558</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>0.908</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>0.618</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>0.974</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>0.841</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
         <is>
           <t>0.840</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="C68" t="inlineStr">
         <is>
           <t>0.588</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="D68" t="inlineStr">
         <is>
           <t>0.828</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="E68" t="inlineStr">
         <is>
           <t>0.629</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="F68" t="inlineStr">
         <is>
           <t>0.982</t>
         </is>

</xml_diff>

<commit_message>
modify the DG_rotation_jigsaw_trainer to have different weight for rotation and jigsaw.
</commit_message>
<xml_diff>
--- a/scripts/result.xlsx
+++ b/scripts/result.xlsx
@@ -345,7 +345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -356,7 +356,7 @@
     <row r="1">
       <c r="B1" t="inlineStr">
         <is>
-          <t>0.4_0.8</t>
+          <t>0.2_0.4</t>
         </is>
       </c>
     </row>
@@ -385,73 +385,73 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>0.687</t>
+          <t>0.694</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>0.686</t>
+          <t>0.711</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>0.570</t>
+          <t>0.645</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>0.901</t>
+          <t>0.887</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>0.689</t>
+          <t>0.675</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>0.705</t>
+          <t>0.695</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0.663</t>
+          <t>0.640</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.899</t>
+          <t>0.905</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>0.678</t>
+          <t>0.663</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>0.713</t>
+          <t>0.707</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.610</t>
+          <t>0.633</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.905</t>
+          <t>0.889</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="B8" t="inlineStr">
         <is>
-          <t>0.4_0.9</t>
+          <t>0.3_0.4</t>
         </is>
       </c>
     </row>
@@ -480,34 +480,34 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>0.673</t>
+          <t>0.696</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>0.694</t>
+          <t>0.705</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>0.619</t>
+          <t>0.674</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>0.883</t>
+          <t>0.889</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>0.690</t>
+          <t>0.699</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>0.697</t>
+          <t>0.684</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -517,36 +517,36 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0.908</t>
+          <t>0.889</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>0.663</t>
+          <t>0.700</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>0.684</t>
+          <t>0.704</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>0.636</t>
+          <t>0.641</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>0.893</t>
+          <t>0.889</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="B15" t="inlineStr">
         <is>
-          <t>0.4_1.0</t>
+          <t>0.4_0.4</t>
         </is>
       </c>
     </row>
@@ -566,82 +566,550 @@
           <t>ap</t>
         </is>
       </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>ap</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>0.678</t>
+          <t>0.686</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>0.709</t>
+          <t>0.699</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>0.636</t>
+          <t>0.644</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>ap</t>
+          <t>0.904</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>0.670</t>
+          <t>0.685</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>0.698</t>
+          <t>0.695</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>0.640</t>
+          <t>0.651</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>0.892</t>
+          <t>0.899</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
+          <t>0.692</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>0.707</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>0.654</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>0.904</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>0.5_0.4</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>ca</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>ap</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>ap</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>ap</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>0.709</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>0.716</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>0.608</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>0.897</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>0.701</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>0.710</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>0.634</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>0.886</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>0.674</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>0.706</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>0.665</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>0.890</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>0.6_0.4</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>ca</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>ap</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>ap</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>ap</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>0.686</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>0.711</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>0.641</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>0.904</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>0.680</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>0.698</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>0.659</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>0.897</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>0.708</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>0.692</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>0.651</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>0.901</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>0.7_0.4</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>ca</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>ap</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>ap</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>ap</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>0.698</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>0.695</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>0.657</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>0.898</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>0.687</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>0.704</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>0.635</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>0.893</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>0.702</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>0.693</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>0.645</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>0.892</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>0.8_0.4</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>ca</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>ap</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>ap</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>ap</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>0.695</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>0.686</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>0.655</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>0.885</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>0.676</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>0.701</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>0.689</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>0.893</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>0.678</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>0.699</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>0.674</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>0.900</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>0.9_0.4</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>ca</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>ap</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>ap</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>ap</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
           <t>0.684</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>0.709</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>0.633</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>0.899</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>0.620</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>0.898</t>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>0.725</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>0.661</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>0.894</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>0.713</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>0.704</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>0.658</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>0.900</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>0.694</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>0.701</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>0.661</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>0.894</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
add another caffnet model to combine both jigsaw and rotation task.
</commit_message>
<xml_diff>
--- a/scripts/result.xlsx
+++ b/scripts/result.xlsx
@@ -345,7 +345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D54"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -356,7 +356,7 @@
     <row r="1">
       <c r="B1" t="inlineStr">
         <is>
-          <t>0.2_0.4</t>
+          <t>0.85_0.85_0.4</t>
         </is>
       </c>
     </row>
@@ -385,73 +385,73 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>0.694</t>
+          <t>0.672</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>0.711</t>
+          <t>0.702</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>0.645</t>
+          <t>0.677</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>0.887</t>
+          <t>0.893</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>0.675</t>
+          <t>0.677</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>0.695</t>
+          <t>0.710</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0.640</t>
+          <t>0.658</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.905</t>
+          <t>0.892</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>0.663</t>
+          <t>0.689</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>0.707</t>
+          <t>0.702</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.633</t>
+          <t>0.672</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.889</t>
+          <t>0.880</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="B8" t="inlineStr">
         <is>
-          <t>0.3_0.4</t>
+          <t>0.95_0.95_0.4</t>
         </is>
       </c>
     </row>
@@ -480,39 +480,39 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>0.696</t>
+          <t>0.684</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>0.705</t>
+          <t>0.695</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>0.674</t>
+          <t>0.638</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>0.889</t>
+          <t>0.893</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>0.699</t>
+          <t>0.684</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>0.684</t>
+          <t>0.691</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>0.661</t>
+          <t>0.677</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -524,7 +524,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>0.700</t>
+          <t>0.689</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -534,19 +534,19 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>0.641</t>
+          <t>0.607</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>0.889</t>
+          <t>0.893</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="B15" t="inlineStr">
         <is>
-          <t>0.4_0.4</t>
+          <t>0.9_0.9_0.35</t>
         </is>
       </c>
     </row>
@@ -575,73 +575,73 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>0.686</t>
+          <t>0.688</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>0.699</t>
+          <t>0.710</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>0.644</t>
+          <t>0.660</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0.904</t>
+          <t>0.900</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>0.685</t>
+          <t>0.692</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>0.695</t>
+          <t>0.686</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>0.651</t>
+          <t>0.656</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>0.899</t>
+          <t>0.890</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>0.692</t>
+          <t>0.684</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>0.707</t>
+          <t>0.696</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>0.654</t>
+          <t>0.661</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>0.904</t>
+          <t>0.889</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="B22" t="inlineStr">
         <is>
-          <t>0.5_0.4</t>
+          <t>0.9_0.9_0.45</t>
         </is>
       </c>
     </row>
@@ -670,446 +670,66 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>0.709</t>
+          <t>0.683</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>0.716</t>
+          <t>0.699</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>0.608</t>
+          <t>0.646</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>0.897</t>
+          <t>0.886</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>0.701</t>
+          <t>0.682</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>0.710</t>
+          <t>0.689</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>0.634</t>
+          <t>0.632</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>0.886</t>
+          <t>0.887</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>0.674</t>
+          <t>0.694</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>0.706</t>
+          <t>0.693</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>0.665</t>
+          <t>0.663</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>0.890</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>0.6_0.4</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>ca</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>ap</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>ap</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>ap</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>0.686</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>0.711</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>0.641</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>0.904</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>0.680</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>0.698</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>0.659</t>
-        </is>
-      </c>
-      <c r="D32" t="inlineStr">
-        <is>
           <t>0.897</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>0.708</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>0.692</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>0.651</t>
-        </is>
-      </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>0.901</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>0.7_0.4</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>ca</t>
-        </is>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>ap</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>ap</t>
-        </is>
-      </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>ap</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>0.698</t>
-        </is>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>0.695</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>0.657</t>
-        </is>
-      </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>0.898</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>0.687</t>
-        </is>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>0.704</t>
-        </is>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>0.635</t>
-        </is>
-      </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>0.893</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>0.702</t>
-        </is>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>0.693</t>
-        </is>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>0.645</t>
-        </is>
-      </c>
-      <c r="D40" t="inlineStr">
-        <is>
-          <t>0.892</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>0.8_0.4</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>ca</t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>ap</t>
-        </is>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>ap</t>
-        </is>
-      </c>
-      <c r="D44" t="inlineStr">
-        <is>
-          <t>ap</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>0.695</t>
-        </is>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>0.686</t>
-        </is>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>0.655</t>
-        </is>
-      </c>
-      <c r="D45" t="inlineStr">
-        <is>
-          <t>0.885</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>0.676</t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>0.701</t>
-        </is>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>0.689</t>
-        </is>
-      </c>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t>0.893</t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>0.678</t>
-        </is>
-      </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>0.699</t>
-        </is>
-      </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>0.674</t>
-        </is>
-      </c>
-      <c r="D47" t="inlineStr">
-        <is>
-          <t>0.900</t>
-        </is>
-      </c>
-    </row>
-    <row r="50">
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>0.9_0.4</t>
-        </is>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>ca</t>
-        </is>
-      </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>ap</t>
-        </is>
-      </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>ap</t>
-        </is>
-      </c>
-      <c r="D51" t="inlineStr">
-        <is>
-          <t>ap</t>
-        </is>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>0.684</t>
-        </is>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>0.725</t>
-        </is>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>0.661</t>
-        </is>
-      </c>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t>0.894</t>
-        </is>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>0.713</t>
-        </is>
-      </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>0.704</t>
-        </is>
-      </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>0.658</t>
-        </is>
-      </c>
-      <c r="D53" t="inlineStr">
-        <is>
-          <t>0.900</t>
-        </is>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>0.694</t>
-        </is>
-      </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>0.701</t>
-        </is>
-      </c>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t>0.661</t>
-        </is>
-      </c>
-      <c r="D54" t="inlineStr">
-        <is>
-          <t>0.894</t>
         </is>
       </c>
     </row>

</xml_diff>